<commit_message>
Production Release 8th Dev 2022
</commit_message>
<xml_diff>
--- a/Corpus/MLR_Corpus.xlsx
+++ b/Corpus/MLR_Corpus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sivan\Downloads\Masori-Chatbot-UAT-main (3)\Masori-Chatbot-UAT-main\Corpus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SivanSpeed\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C50D03D-4311-497F-BEEF-7DAD4B3718AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F2295B-2054-4519-B493-AE79EBC8BD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Nuplazid HCP" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Nuplazid Consumer'!$A$1:$M$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Nuplazid Consumer'!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Nuplazid HCP'!$A$1:$M$91</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -44,7 +44,7 @@
     <author>tc={97A1DE64-2A59-4152-9781-91195D1F313C}</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{B4468C53-9464-4F63-81D1-C992873261B1}">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{7863A5D1-9B4B-42AA-9E3A-EFD2CA1F4ACC}">
       <text>
         <r>
           <rPr>
@@ -67,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="1" shapeId="0" xr:uid="{DD2E8F32-48A3-491E-956A-AC81F7E38ADB}">
+    <comment ref="C2" authorId="1" shapeId="0" xr:uid="{E64DB1B2-189A-48BC-A2B1-134AFAF4CC9B}">
       <text>
         <r>
           <rPr>
@@ -86,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="2" shapeId="0" xr:uid="{BB84B340-AF06-4E0C-AE4F-B69F85FAF690}">
+    <comment ref="F2" authorId="2" shapeId="0" xr:uid="{7D77409F-1EAA-44C8-96B2-9ED33BE485CA}">
       <text>
         <r>
           <rPr>
@@ -103,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="3" shapeId="0" xr:uid="{C3DFF50C-EF22-47C6-868C-F20870D79A79}">
+    <comment ref="F3" authorId="3" shapeId="0" xr:uid="{7A10A0C6-BB3F-408D-A4EF-B3CB00342EF2}">
       <text>
         <r>
           <rPr>
@@ -120,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="4" shapeId="0" xr:uid="{2B46EE82-DD41-45F9-B431-51F301EDCADE}">
+    <comment ref="F4" authorId="4" shapeId="0" xr:uid="{50AA08B8-0148-4B06-9956-D51213AE6275}">
       <text>
         <r>
           <rPr>
@@ -137,7 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="5" shapeId="0" xr:uid="{190DBEEA-93D9-4BFD-AD5C-1FA3C401F8CC}">
+    <comment ref="B5" authorId="5" shapeId="0" xr:uid="{DFB3A94E-DDA4-466E-AAE1-2757AB1D255D}">
       <text>
         <r>
           <rPr>
@@ -154,7 +154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C15" authorId="6" shapeId="0" xr:uid="{6174D911-122C-4454-8324-AF7C643C4042}">
+    <comment ref="C15" authorId="6" shapeId="0" xr:uid="{94516435-0266-4ADB-BEEF-4CB81A803132}">
       <text>
         <r>
           <rPr>
@@ -171,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D25" authorId="7" shapeId="0" xr:uid="{C6BC059E-DDFE-4471-8AF3-B08E62FA3401}">
+    <comment ref="D25" authorId="7" shapeId="0" xr:uid="{422F338D-F43C-4C76-95CA-BE3FA3F1C9BA}">
       <text>
         <r>
           <rPr>
@@ -188,7 +188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E27" authorId="8" shapeId="0" xr:uid="{97A1DE64-2A59-4152-9781-91195D1F313C}">
+    <comment ref="E27" authorId="8" shapeId="0" xr:uid="{6E745FC6-AE79-477C-95B8-95241C30BDC2}">
       <text>
         <r>
           <rPr>
@@ -407,7 +407,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="344">
   <si>
     <t>Keywords</t>
   </si>
@@ -1606,9 +1606,6 @@
     <t xml:space="preserve">For any Medical questions or comments please contact Medical Information: </t>
   </si>
   <si>
-    <t>For any specific medical questions, comments, or concerns, please contact Medical Affairs team:</t>
-  </si>
-  <si>
     <t>Email : medicalinformation@acadia-pharm.com
 Phone : 1-844-4ACADIA&lt;br&gt;(1-844-422-2342)</t>
   </si>
@@ -1617,8 +1614,13 @@
 Phone: 1-844-4ACADIA&lt;br&gt;(1-844-422-2342)</t>
   </si>
   <si>
-    <t>If you have experienced an adverse event or have a product complaint, contact Acadia Pharmaceuticals at
-1-800-4ACADIA (1-844-422-2342)</t>
+    <t>If you have experienced an adverse event or have a product complaint, contact Acadia Pharmaceuticals at 1-800-4ACADIA&lt;br&gt;(1-844-422-2342)</t>
+  </si>
+  <si>
+    <t>HCPFinder</t>
+  </si>
+  <si>
+    <t>/resources#FindSpecialist</t>
   </si>
 </sst>
 </file>
@@ -1764,24 +1766,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1789,20 +1791,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2181,7 +2183,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A4"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2241,14 +2243,14 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
         <v>200</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="22" t="s">
         <v>242</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -2266,14 +2268,14 @@
       <c r="L2" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="M2" s="27" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
@@ -2289,12 +2291,12 @@
       <c r="L3" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="M3" s="22"/>
+      <c r="M3" s="25"/>
     </row>
     <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
       <c r="D4" s="1" t="s">
         <v>292</v>
       </c>
@@ -2310,16 +2312,16 @@
       <c r="L4" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="M4" s="22"/>
-    </row>
-    <row r="5" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
+      <c r="M4" s="25"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="21" t="s">
         <v>251</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="21" t="s">
         <v>205</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -2337,14 +2339,14 @@
       <c r="L5" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="M5" s="23" t="s">
+      <c r="M5" s="24" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="1" t="s">
         <v>274</v>
       </c>
@@ -2360,16 +2362,16 @@
       <c r="L6" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="M6" s="22"/>
-    </row>
-    <row r="7" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
+      <c r="M6" s="25"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="21" t="s">
         <v>256</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="21" t="s">
         <v>259</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -2387,14 +2389,14 @@
       <c r="L7" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="M7" s="23" t="s">
+      <c r="M7" s="24" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="1" t="s">
         <v>258</v>
       </c>
@@ -2410,16 +2412,15 @@
       <c r="L8" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="M8" s="22"/>
+      <c r="M8" s="25"/>
     </row>
     <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E9"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -2429,18 +2430,17 @@
       <c r="L9" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="M9" s="22"/>
+      <c r="M9" s="25"/>
     </row>
     <row r="10" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="E10"/>
       <c r="F10" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -2463,7 +2463,6 @@
       <c r="D11" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="E11"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="15"/>
@@ -2481,8 +2480,6 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12"/>
-      <c r="E12"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -2496,8 +2493,6 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13"/>
-      <c r="E13"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -2511,8 +2506,6 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14"/>
-      <c r="E14"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -2522,14 +2515,14 @@
       <c r="L14" s="1"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="1:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="24" t="s">
+    <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="21" t="s">
         <v>252</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -2547,14 +2540,14 @@
       <c r="L15" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="M15" s="23" t="s">
+      <c r="M15" s="24" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
       <c r="D16" s="1" t="s">
         <v>295</v>
       </c>
@@ -2570,12 +2563,12 @@
       <c r="L16" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="M16" s="22"/>
+      <c r="M16" s="25"/>
     </row>
     <row r="17" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="1" t="s">
         <v>296</v>
       </c>
@@ -2591,12 +2584,12 @@
       <c r="L17" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="M17" s="22"/>
+      <c r="M17" s="25"/>
     </row>
     <row r="18" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="24"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
       <c r="D18" s="1" t="s">
         <v>301</v>
       </c>
@@ -2604,22 +2597,20 @@
         <v>66</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="G18" s="1" t="s">
         <v>341</v>
       </c>
+      <c r="G18" s="1"/>
       <c r="L18" s="15"/>
-      <c r="M18" s="22"/>
-    </row>
-    <row r="19" spans="1:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="24" t="s">
+      <c r="M18" s="25"/>
+    </row>
+    <row r="19" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="21" t="s">
         <v>208</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -2637,14 +2628,14 @@
       <c r="L19" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="M19" s="23" t="s">
+      <c r="M19" s="24" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="24"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="24"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="23"/>
       <c r="D20" s="1" t="s">
         <v>298</v>
       </c>
@@ -2660,12 +2651,12 @@
       <c r="L20" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="M20" s="22"/>
+      <c r="M20" s="25"/>
     </row>
     <row r="21" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="24"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="24"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="23"/>
       <c r="D21" s="1" t="s">
         <v>175</v>
       </c>
@@ -2681,12 +2672,12 @@
       <c r="L21" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="M21" s="22"/>
+      <c r="M21" s="25"/>
     </row>
     <row r="22" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="24"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="24"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="23"/>
       <c r="D22" s="1" t="s">
         <v>176</v>
       </c>
@@ -2702,22 +2693,21 @@
       <c r="L22" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="M22" s="22"/>
-    </row>
-    <row r="23" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="24" t="s">
+      <c r="M22" s="25"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="21" t="s">
         <v>209</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="E23"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -2727,14 +2717,14 @@
       <c r="L23" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="M23" s="23" t="s">
+      <c r="M23" s="24" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="24"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="24"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="23"/>
       <c r="D24" s="1" t="s">
         <v>18</v>
       </c>
@@ -2750,12 +2740,12 @@
       <c r="L24" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="M24" s="22"/>
+      <c r="M24" s="25"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="24"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="24"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="23"/>
       <c r="D25" s="1" t="s">
         <v>254</v>
       </c>
@@ -2770,12 +2760,12 @@
       <c r="L25" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="M25" s="22"/>
+      <c r="M25" s="25"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="24"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="24"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="23"/>
       <c r="D26" s="1" t="s">
         <v>66</v>
       </c>
@@ -2791,13 +2781,13 @@
       <c r="L26" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="M26" s="22"/>
-    </row>
-    <row r="27" spans="1:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="24" t="s">
+      <c r="M26" s="25"/>
+    </row>
+    <row r="27" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="21" t="s">
         <v>210</v>
       </c>
       <c r="C27" s="26" t="s">
@@ -2817,13 +2807,13 @@
       <c r="L27" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="M27" s="23" t="s">
+      <c r="M27" s="24" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="24"/>
-      <c r="B28" s="25"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="21"/>
       <c r="C28" s="26"/>
       <c r="D28" s="1" t="s">
         <v>179</v>
@@ -2840,49 +2830,44 @@
       <c r="L28" s="15" t="s">
         <v>319</v>
       </c>
-      <c r="M28" s="22"/>
+      <c r="M28" s="25"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="24"/>
-      <c r="B29" s="25"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="26"/>
-      <c r="D29"/>
-      <c r="E29"/>
       <c r="L29" s="19" t="s">
         <v>319</v>
       </c>
-      <c r="M29" s="22"/>
+      <c r="M29" s="25"/>
     </row>
     <row r="30" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="E30"/>
       <c r="F30" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="G30" s="1" t="s">
         <v>341</v>
       </c>
+      <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="15"/>
-      <c r="M30" s="23" t="s">
+      <c r="M30" s="24" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="24"/>
-      <c r="B31" s="25" t="s">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="23"/>
+      <c r="B31" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="21" t="s">
         <v>213</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -2900,37 +2885,35 @@
       <c r="L31" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="M31" s="22"/>
+      <c r="M31" s="25"/>
     </row>
     <row r="32" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="24"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="25"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="21"/>
       <c r="D32" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="E32"/>
       <c r="F32" s="1" t="s">
         <v>337</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="15"/>
-      <c r="M32" s="22"/>
+      <c r="M32" s="25"/>
     </row>
     <row r="33" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="24"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="25"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="21"/>
       <c r="D33" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="E33"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -2940,12 +2923,12 @@
       <c r="L33" s="15" t="s">
         <v>327</v>
       </c>
-      <c r="M33" s="22"/>
+      <c r="M33" s="25"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34" s="24"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="25"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="21"/>
       <c r="D34" s="1" t="s">
         <v>172</v>
       </c>
@@ -2961,12 +2944,12 @@
       <c r="L34" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="M34" s="22"/>
+      <c r="M34" s="25"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A35" s="24"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="25"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="21"/>
       <c r="D35" s="1" t="s">
         <v>202</v>
       </c>
@@ -2982,16 +2965,15 @@
       <c r="L35" s="15" t="s">
         <v>327</v>
       </c>
-      <c r="M35" s="22"/>
+      <c r="M35" s="25"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A36" s="24"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="25"/>
+      <c r="A36" s="23"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="21"/>
       <c r="D36" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E36"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -3001,16 +2983,16 @@
       <c r="L36" s="15" t="s">
         <v>327</v>
       </c>
-      <c r="M36" s="22"/>
-    </row>
-    <row r="37" spans="1:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="25" t="s">
+      <c r="M36" s="25"/>
+    </row>
+    <row r="37" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="B37" s="25" t="s">
+      <c r="B37" s="21" t="s">
         <v>215</v>
       </c>
-      <c r="C37" s="25" t="s">
+      <c r="C37" s="21" t="s">
         <v>216</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -3028,14 +3010,14 @@
       <c r="L37" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="M37" s="23" t="s">
+      <c r="M37" s="24" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="25"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="24"/>
+      <c r="A38" s="21"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="23"/>
       <c r="D38" s="1" t="s">
         <v>182</v>
       </c>
@@ -3051,39 +3033,37 @@
       <c r="L38" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="M38" s="22"/>
+      <c r="M38" s="25"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A39" s="25"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="24"/>
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="23"/>
       <c r="D39" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E39"/>
       <c r="F39" s="15"/>
       <c r="L39" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="M39" s="22"/>
+      <c r="M39" s="25"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A40" s="25"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="24"/>
+      <c r="A40" s="21"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="23"/>
       <c r="D40" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E40"/>
       <c r="L40" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="M40" s="22"/>
+      <c r="M40" s="25"/>
     </row>
     <row r="41" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="25"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="24"/>
+      <c r="A41" s="21"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="23"/>
       <c r="D41" s="1" t="s">
         <v>185</v>
       </c>
@@ -3099,12 +3079,12 @@
       <c r="L41" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="M41" s="22"/>
+      <c r="M41" s="25"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A42" s="25"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="24"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="23"/>
       <c r="D42" s="1" t="s">
         <v>277</v>
       </c>
@@ -3120,12 +3100,12 @@
       <c r="L42" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="M42" s="22"/>
+      <c r="M42" s="25"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A43" s="25"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="24"/>
+      <c r="A43" s="21"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="23"/>
       <c r="D43" s="1" t="s">
         <v>187</v>
       </c>
@@ -3141,13 +3121,11 @@
       <c r="L43" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="M43" s="22"/>
+      <c r="M43" s="25"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
-      <c r="D44"/>
-      <c r="E44"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
@@ -3182,26 +3160,24 @@
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D46"/>
-      <c r="L46" s="15"/>
+      <c r="A46" t="s">
+        <v>342</v>
+      </c>
+      <c r="D46" t="s">
+        <v>342</v>
+      </c>
+      <c r="L46" s="15" t="s">
+        <v>343</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A37:A43"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="B31:B36"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B37:B43"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C31:C36"/>
-    <mergeCell ref="C37:C43"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="M30:M36"/>
-    <mergeCell ref="M37:M43"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M15:M18"/>
+    <mergeCell ref="M19:M22"/>
+    <mergeCell ref="M23:M26"/>
+    <mergeCell ref="M7:M9"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="B5:B6"/>
@@ -3210,67 +3186,76 @@
     <mergeCell ref="C15:C18"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="C7:C10"/>
+    <mergeCell ref="C31:C36"/>
+    <mergeCell ref="C37:C43"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="M30:M36"/>
+    <mergeCell ref="M37:M43"/>
+    <mergeCell ref="M27:M29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B37:B43"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="A37:A43"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A15:A18"/>
     <mergeCell ref="A19:A22"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="A7:A10"/>
-    <mergeCell ref="M27:M29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M15:M18"/>
-    <mergeCell ref="M19:M22"/>
-    <mergeCell ref="M23:M26"/>
-    <mergeCell ref="M7:M9"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="M5" r:id="rId2" display="https://www.nuplazid.com/about-nuplazid" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="M15" r:id="rId3" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="M19" r:id="rId4" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="M23" r:id="rId5" display="https://www.nuplazid.com/contact-us" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="M27" r:id="rId6" display="https://www.nuplazid.com/" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="M30" r:id="rId7" display="https://www.nuplazid.com/frequently-asked-questions" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="M37" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="M45" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="M7" r:id="rId10" display="https://nuplazid-masori.azurewebsites.net/talking-to-your-healthcare-provider" xr:uid="{4E0AA375-15F4-4928-90C2-BD2E1EC884AB}"/>
-    <hyperlink ref="M11" r:id="rId11" display="https://www.nuplazid.com/personal-stories" xr:uid="{E29A4A0F-3BAA-48B7-B469-0201A35D0289}"/>
-    <hyperlink ref="L2" r:id="rId12" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{4495FBCE-2467-41F6-83E7-F374F4E5ACAB}"/>
-    <hyperlink ref="L3" r:id="rId13" location="doctor-discussion-guide" display="https://nuplazid-masori.azurewebsites.net/talking-to-your-healthcare-provider#doctor-discussion-guide" xr:uid="{75D08F74-8D31-42CD-9DEA-EB3C155B058E}"/>
-    <hyperlink ref="L4" r:id="rId14" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{24EA9806-C569-4951-9504-2FBC155A4446}"/>
-    <hyperlink ref="L5" r:id="rId15" display="https://www.nuplazid.com/about-nuplazid" xr:uid="{B2640193-23B3-4108-9FF7-9A01FDC2AAC4}"/>
-    <hyperlink ref="L6" r:id="rId16" display="https://www.nuplazid.com/about-nuplazid" xr:uid="{4F3333E6-215D-49C2-B203-B676F10F4601}"/>
-    <hyperlink ref="L7" r:id="rId17" location="doctor-discussion-guide" display="https://www.nuplazid.com/talking-to-your-healthcare-provider#doctor-discussion-guide" xr:uid="{6990F5E4-6310-4A17-B71D-FAB7F93D11D5}"/>
-    <hyperlink ref="L8" r:id="rId18" display="https://www.nuplazid.com/talking-to-your-healthcare-provider" xr:uid="{04233E34-718D-4FD2-B60C-142BE08A93EF}"/>
-    <hyperlink ref="L9" r:id="rId19" display="https://www.nuplazid.com/talking-to-your-healthcare-provider" xr:uid="{F743F447-69D3-44E6-A171-3A5CDB40140F}"/>
-    <hyperlink ref="L11" r:id="rId20" display="https://www.nuplazid.com/personal-stories" xr:uid="{C74AC20C-A05F-45CF-9703-88D2A8AD3FA3}"/>
-    <hyperlink ref="L15" r:id="rId21" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{703ADCC4-AC29-4435-B772-0DCE375018AF}"/>
-    <hyperlink ref="L16" r:id="rId22" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{56E5B06F-C1CB-4447-8CED-900F308AED36}"/>
-    <hyperlink ref="L17" r:id="rId23" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{166ECE66-73AB-4DBD-9A5D-F709522CA032}"/>
-    <hyperlink ref="L19" r:id="rId24" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{78C775ED-2F8D-4D3F-9F9B-5A6828934667}"/>
-    <hyperlink ref="L20" r:id="rId25" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{CD1EEE7E-824A-4F08-B602-3ED6D1A8389D}"/>
-    <hyperlink ref="L21" r:id="rId26" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{8640B23A-0564-4B4D-B884-8335E9443CE5}"/>
-    <hyperlink ref="L22" r:id="rId27" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{D87217C7-4000-4C28-BE83-BC0F9F5A6DAB}"/>
-    <hyperlink ref="L23" r:id="rId28" display="https://www.nuplazid.com/contact-us" xr:uid="{F2924CF2-7E96-423B-AB36-C38EAA415835}"/>
-    <hyperlink ref="L28" r:id="rId29" display="https://www.nuplazid.com/" xr:uid="{20DF50FF-9FE4-4468-9A0E-F46415473F00}"/>
-    <hyperlink ref="L29" r:id="rId30" display="https://www.nuplazid.com/" xr:uid="{59F18694-A2C4-4EAC-B6DE-07FB3F72DBE8}"/>
-    <hyperlink ref="L33" r:id="rId31" display="https://www.nuplazid.com/frequently-asked-questions" xr:uid="{6B467D41-7205-4A17-BD9B-3069472F3D20}"/>
-    <hyperlink ref="L35" r:id="rId32" display="https://www.nuplazid.com/frequently-asked-questions" xr:uid="{7ADE210C-D0C7-47F2-958D-6D2416CE6200}"/>
-    <hyperlink ref="L36" r:id="rId33" display="https://www.nuplazid.com/frequently-asked-questions" xr:uid="{B3CCBC56-1DC9-4339-86D0-D43726FFFF53}"/>
-    <hyperlink ref="L45" r:id="rId34" display="https://www.acadiaconnect.com/patient-caregivers" xr:uid="{73DAF1B1-3B43-4FD4-9161-2EE6FA67CE88}"/>
-    <hyperlink ref="L27" r:id="rId35" display="https://www.nuplazid.com/pdf/nuplazid-prescribing-information.pdf" xr:uid="{A989EB85-40E9-492E-BB74-5DDDBB25F0A2}"/>
-    <hyperlink ref="L43" r:id="rId36" display="https://nuplazid-masori.azurewebsites.net/support-and-resources" xr:uid="{52D7B43E-E1C5-452E-800C-55136E47BFD5}"/>
-    <hyperlink ref="L42" r:id="rId37" display="https://nuplazid-masori.azurewebsites.net/resources" xr:uid="{8648DAD8-AEA8-454E-99EF-DFF9F0B9F3B2}"/>
-    <hyperlink ref="L41" r:id="rId38" display="https://nuplazid-masori.azurewebsites.net/support-and-resources" xr:uid="{0C802C3D-BF63-47DF-88E7-3650A6DBE099}"/>
-    <hyperlink ref="L25" r:id="rId39" display="https://www.nuplazid.com/contact-us" xr:uid="{64FBF0F2-0B60-4F14-90A6-0F8CBA9FA3C9}"/>
-    <hyperlink ref="L26" r:id="rId40" display="https://nuplazid-masori.azurewebsites.net/safety-information" xr:uid="{F9138170-4EC6-4548-8402-78546A70D6B6}"/>
-    <hyperlink ref="L34" r:id="rId41" display="https://nuplazid-masori.azurewebsites.net/about-nuplazid" xr:uid="{2DAD216E-8CE3-4828-AE30-B57254452928}"/>
-    <hyperlink ref="L31" r:id="rId42" display="https://nuplazid-masori.azurewebsites.net/about-nuplazid" xr:uid="{43B11A0D-DCBC-4AD4-9F17-2751B459B294}"/>
-    <hyperlink ref="L37" r:id="rId43" display="https://nuplazid-masori.azurewebsites.net/support-and-resources" xr:uid="{D342507B-3D19-49A1-93B0-C3FDAA7E51FC}"/>
-    <hyperlink ref="L38" r:id="rId44" display="https://nuplazid-masori.azurewebsites.net/support-and-resources" xr:uid="{A256E305-D2BB-4447-8040-2212C8028B71}"/>
-    <hyperlink ref="L39" r:id="rId45" display="https://nuplazid-masori.azurewebsites.net/support-and-resources" xr:uid="{E8484EE3-FEBC-4129-BFC7-760311475612}"/>
-    <hyperlink ref="L24" r:id="rId46" display="https://www.nuplazid.com/about-nuplazid" xr:uid="{D9A18C26-D7E7-4D8D-919E-B4D043966A2B}"/>
+    <hyperlink ref="M2" r:id="rId1" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{8B199CA5-51D2-4A5F-A317-094F7584A959}"/>
+    <hyperlink ref="M5" r:id="rId2" display="https://www.nuplazid.com/about-nuplazid" xr:uid="{32F0AB5C-DA1B-41ED-9FB3-54209BD30C44}"/>
+    <hyperlink ref="M15" r:id="rId3" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{76406452-9A96-4265-83E8-3E7715DEE15F}"/>
+    <hyperlink ref="M19" r:id="rId4" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{543B42DC-7774-4DE0-B9BE-F131EA21418F}"/>
+    <hyperlink ref="M23" r:id="rId5" display="https://www.nuplazid.com/contact-us" xr:uid="{5250991C-CB2A-4F23-9D0B-4AB0D2A2E3A7}"/>
+    <hyperlink ref="M27" r:id="rId6" display="https://www.nuplazid.com/" xr:uid="{CF432552-ED2E-4C35-83A6-FF9A60F7C736}"/>
+    <hyperlink ref="M30" r:id="rId7" display="https://www.nuplazid.com/frequently-asked-questions" xr:uid="{D4FB2B85-E6E6-471A-B99B-E292493DC976}"/>
+    <hyperlink ref="M37" r:id="rId8" xr:uid="{3405A261-7A1A-4364-8AC1-25AE754A0A00}"/>
+    <hyperlink ref="M45" r:id="rId9" xr:uid="{67D6A31F-0688-4D03-99D4-F90BEBFE4CDA}"/>
+    <hyperlink ref="M7" r:id="rId10" display="https://nuplazid-masori.azurewebsites.net/talking-to-your-healthcare-provider" xr:uid="{8508225C-113C-4D74-9419-6F19C697270A}"/>
+    <hyperlink ref="M11" r:id="rId11" display="https://www.nuplazid.com/personal-stories" xr:uid="{928F4EA1-A837-48EE-8D41-B83B80620299}"/>
+    <hyperlink ref="L2" r:id="rId12" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{6140476F-70BA-416A-9672-0BB7500BC5EE}"/>
+    <hyperlink ref="L3" r:id="rId13" location="doctor-discussion-guide" display="https://nuplazid-masori.azurewebsites.net/talking-to-your-healthcare-provider#doctor-discussion-guide" xr:uid="{5F9A82C5-F8BA-4534-9250-4366A0C5F7EC}"/>
+    <hyperlink ref="L4" r:id="rId14" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{DB975650-2175-41C0-A382-DE720812DECF}"/>
+    <hyperlink ref="L5" r:id="rId15" display="https://www.nuplazid.com/about-nuplazid" xr:uid="{E44B7DB3-1B45-4F92-A9CA-7452B96DE72C}"/>
+    <hyperlink ref="L6" r:id="rId16" display="https://www.nuplazid.com/about-nuplazid" xr:uid="{69FC6AC5-D419-4098-B1AE-4D44D7B72B87}"/>
+    <hyperlink ref="L7" r:id="rId17" location="doctor-discussion-guide" display="https://www.nuplazid.com/talking-to-your-healthcare-provider#doctor-discussion-guide" xr:uid="{F1F00104-1051-42F8-BBE0-47FF161820A2}"/>
+    <hyperlink ref="L8" r:id="rId18" display="https://www.nuplazid.com/talking-to-your-healthcare-provider" xr:uid="{6AC1B59F-76B0-4242-8276-7D4CA1713A2A}"/>
+    <hyperlink ref="L9" r:id="rId19" display="https://www.nuplazid.com/talking-to-your-healthcare-provider" xr:uid="{B2943157-7C8D-4EF6-8B34-1FD3DEF8999A}"/>
+    <hyperlink ref="L11" r:id="rId20" display="https://www.nuplazid.com/personal-stories" xr:uid="{F818F6ED-3242-4C86-89C5-BD0844207BA9}"/>
+    <hyperlink ref="L15" r:id="rId21" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{E23CADA4-C42E-4EB3-BE76-65E7B733438E}"/>
+    <hyperlink ref="L16" r:id="rId22" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{736462E8-D8E2-4ABA-998E-929DC73E2199}"/>
+    <hyperlink ref="L17" r:id="rId23" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{16B2C520-5FA2-44E4-83C1-F7254FB8A33D}"/>
+    <hyperlink ref="L19" r:id="rId24" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{A2B621BB-3BF1-41F8-A429-BA1D7B4CBBD6}"/>
+    <hyperlink ref="L20" r:id="rId25" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{29046AFB-F042-4C19-8032-B08C841FF9D3}"/>
+    <hyperlink ref="L21" r:id="rId26" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{23BE0984-F947-4300-97DF-EB83631D2037}"/>
+    <hyperlink ref="L22" r:id="rId27" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{4BABF519-DDEA-4085-8CB3-3468C20FC140}"/>
+    <hyperlink ref="L23" r:id="rId28" display="https://www.nuplazid.com/contact-us" xr:uid="{4EE3C5D7-AC27-4D42-9A0D-B2E0E36EDF5A}"/>
+    <hyperlink ref="L28" r:id="rId29" display="https://www.nuplazid.com/" xr:uid="{EE744E74-5329-4339-BA28-4554A0AD4B19}"/>
+    <hyperlink ref="L29" r:id="rId30" display="https://www.nuplazid.com/" xr:uid="{BE34B179-0AD1-4C55-9B78-62AE88340179}"/>
+    <hyperlink ref="L33" r:id="rId31" display="https://www.nuplazid.com/frequently-asked-questions" xr:uid="{B3DCB349-B5C5-44A1-BA4D-31F9AF688096}"/>
+    <hyperlink ref="L35" r:id="rId32" display="https://www.nuplazid.com/frequently-asked-questions" xr:uid="{9EC3757D-B977-418E-9CD6-2D671BBF91F9}"/>
+    <hyperlink ref="L36" r:id="rId33" display="https://www.nuplazid.com/frequently-asked-questions" xr:uid="{0940F6F4-9166-49EF-8FAC-2B3D661C4CA5}"/>
+    <hyperlink ref="L45" r:id="rId34" display="https://www.acadiaconnect.com/patient-caregivers" xr:uid="{61938416-9C9E-43F7-BCB6-FBF2519B56AA}"/>
+    <hyperlink ref="L27" r:id="rId35" display="https://www.nuplazid.com/pdf/nuplazid-prescribing-information.pdf" xr:uid="{CCE4E02C-7EE9-436A-AB7E-74ACF281740C}"/>
+    <hyperlink ref="L43" r:id="rId36" display="https://nuplazid-masori.azurewebsites.net/support-and-resources" xr:uid="{826542AF-D86B-48E6-8CA6-9FFA96C5B341}"/>
+    <hyperlink ref="L42" r:id="rId37" display="https://nuplazid-masori.azurewebsites.net/resources" xr:uid="{45E3F677-CD33-4D16-A512-1E2964AD6E67}"/>
+    <hyperlink ref="L41" r:id="rId38" display="https://nuplazid-masori.azurewebsites.net/support-and-resources" xr:uid="{899A391F-494B-4BFB-912E-15EF1269BE60}"/>
+    <hyperlink ref="L25" r:id="rId39" display="https://www.nuplazid.com/contact-us" xr:uid="{1B9BE8C7-42E4-4DB5-A7C2-7A49A8904372}"/>
+    <hyperlink ref="L26" r:id="rId40" display="https://nuplazid-masori.azurewebsites.net/safety-information" xr:uid="{6D1F72EE-D0A0-429D-900B-155D31B94D6E}"/>
+    <hyperlink ref="L34" r:id="rId41" display="https://nuplazid-masori.azurewebsites.net/about-nuplazid" xr:uid="{9DC7FFA3-E365-4F60-B1BF-64A08995B2EB}"/>
+    <hyperlink ref="L31" r:id="rId42" display="https://nuplazid-masori.azurewebsites.net/about-nuplazid" xr:uid="{A13B4494-04E8-4EB4-A7AB-5A4D3F818616}"/>
+    <hyperlink ref="L37" r:id="rId43" display="https://nuplazid-masori.azurewebsites.net/support-and-resources" xr:uid="{849EA465-D97C-4C54-9D1A-05392CA141C9}"/>
+    <hyperlink ref="L38" r:id="rId44" display="https://nuplazid-masori.azurewebsites.net/support-and-resources" xr:uid="{0D491D3F-E7A9-4E62-B16A-C4F8E2EDDEB8}"/>
+    <hyperlink ref="L39" r:id="rId45" display="https://nuplazid-masori.azurewebsites.net/support-and-resources" xr:uid="{EF8228C6-48BD-4E1D-8BE4-A1C489D96D3E}"/>
+    <hyperlink ref="L24" r:id="rId46" display="https://www.nuplazid.com/about-nuplazid" xr:uid="{0E8D5C8A-10B2-4AF8-BA4B-CE50B748D3DF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId47"/>
@@ -4381,7 +4366,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="33" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="28" t="s">
@@ -4410,7 +4395,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31"/>
+      <c r="A3" s="34"/>
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
       <c r="D3" s="1" t="s">
@@ -4440,13 +4425,13 @@
       <c r="C4" s="26" t="s">
         <v>241</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="21" t="s">
         <v>302</v>
       </c>
-      <c r="F4" s="25"/>
+      <c r="F4" s="21"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -4455,7 +4440,7 @@
       <c r="L4" s="15" t="s">
         <v>319</v>
       </c>
-      <c r="M4" s="23" t="s">
+      <c r="M4" s="24" t="s">
         <v>319</v>
       </c>
     </row>
@@ -4463,9 +4448,9 @@
       <c r="A5" s="29"/>
       <c r="B5" s="26"/>
       <c r="C5" s="26"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -4474,15 +4459,15 @@
       <c r="L5" s="15" t="s">
         <v>319</v>
       </c>
-      <c r="M5" s="22"/>
+      <c r="M5" s="25"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="29"/>
       <c r="B6" s="26"/>
       <c r="C6" s="26"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -4491,15 +4476,15 @@
       <c r="L6" s="15" t="s">
         <v>319</v>
       </c>
-      <c r="M6" s="22"/>
+      <c r="M6" s="25"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="29"/>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -4508,15 +4493,15 @@
       <c r="L7" s="15" t="s">
         <v>319</v>
       </c>
-      <c r="M7" s="22"/>
+      <c r="M7" s="25"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="29"/>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -4525,7 +4510,7 @@
       <c r="L8" s="15" t="s">
         <v>319</v>
       </c>
-      <c r="M8" s="22"/>
+      <c r="M8" s="25"/>
     </row>
     <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="29"/>
@@ -4554,64 +4539,64 @@
       <c r="A10" s="29" t="s">
         <v>191</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="30" t="s">
         <v>275</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>245</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="21" t="s">
         <v>303</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="21" t="s">
         <v>284</v>
       </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="32" t="s">
+      <c r="F10" s="21"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="31" t="s">
         <v>310</v>
       </c>
-      <c r="M10" s="23" t="s">
+      <c r="M10" s="24" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29"/>
-      <c r="B11" s="25"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="26"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="22"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="25"/>
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29"/>
-      <c r="B12" s="25"/>
+      <c r="B12" s="21"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="22"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="25"/>
     </row>
     <row r="13" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="29"/>
-      <c r="B13" s="25"/>
+      <c r="B13" s="21"/>
       <c r="C13" s="26"/>
       <c r="D13" s="1" t="s">
         <v>334</v>
@@ -4628,11 +4613,11 @@
       <c r="L13" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="M13" s="22"/>
+      <c r="M13" s="25"/>
     </row>
     <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="29"/>
-      <c r="B14" s="25"/>
+      <c r="B14" s="21"/>
       <c r="C14" s="26"/>
       <c r="D14" s="1" t="s">
         <v>29</v>
@@ -4649,11 +4634,11 @@
       <c r="L14" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="M14" s="22"/>
+      <c r="M14" s="25"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="29"/>
-      <c r="B15" s="25"/>
+      <c r="B15" s="21"/>
       <c r="C15" s="26"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -4664,11 +4649,11 @@
       <c r="J15" s="15"/>
       <c r="K15" s="1"/>
       <c r="L15" s="15"/>
-      <c r="M15" s="22"/>
+      <c r="M15" s="25"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="29"/>
-      <c r="B16" s="25"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="26"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -4679,7 +4664,7 @@
       <c r="J16" s="15"/>
       <c r="K16" s="1"/>
       <c r="L16" s="15"/>
-      <c r="M16" s="22"/>
+      <c r="M16" s="25"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
@@ -4700,7 +4685,7 @@
       <c r="J17" s="15"/>
       <c r="K17" s="1"/>
       <c r="L17" s="15"/>
-      <c r="M17" s="23" t="s">
+      <c r="M17" s="24" t="s">
         <v>310</v>
       </c>
     </row>
@@ -4717,7 +4702,7 @@
       <c r="J18" s="15"/>
       <c r="K18" s="1"/>
       <c r="L18" s="15"/>
-      <c r="M18" s="23"/>
+      <c r="M18" s="24"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="29"/>
@@ -4729,7 +4714,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="15"/>
       <c r="L19" s="15"/>
-      <c r="M19" s="23"/>
+      <c r="M19" s="24"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="29"/>
@@ -4744,7 +4729,7 @@
       <c r="J20" s="15"/>
       <c r="K20" s="1"/>
       <c r="L20" s="15"/>
-      <c r="M20" s="23"/>
+      <c r="M20" s="24"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="29"/>
@@ -4763,7 +4748,7 @@
       <c r="L21" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="M21" s="23"/>
+      <c r="M21" s="24"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="29"/>
@@ -4784,7 +4769,7 @@
       <c r="L22" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="M22" s="23"/>
+      <c r="M22" s="24"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="29"/>
@@ -4800,7 +4785,7 @@
       <c r="L23" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="M23" s="23"/>
+      <c r="M23" s="24"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="29"/>
@@ -4821,7 +4806,7 @@
       <c r="L24" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="M24" s="23"/>
+      <c r="M24" s="24"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="29"/>
@@ -4838,7 +4823,7 @@
       <c r="L25" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="M25" s="23"/>
+      <c r="M25" s="24"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="26" t="s">
@@ -4857,7 +4842,7 @@
       <c r="J26" s="15"/>
       <c r="K26" s="1"/>
       <c r="L26" s="15"/>
-      <c r="M26" s="23" t="s">
+      <c r="M26" s="24" t="s">
         <v>310</v>
       </c>
     </row>
@@ -4880,7 +4865,7 @@
       <c r="L27" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="M27" s="22"/>
+      <c r="M27" s="25"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="26"/>
@@ -4896,7 +4881,7 @@
       <c r="L28" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="M28" s="22"/>
+      <c r="M28" s="25"/>
     </row>
     <row r="29" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="26"/>
@@ -4917,7 +4902,7 @@
       <c r="L29" s="15" t="s">
         <v>311</v>
       </c>
-      <c r="M29" s="22"/>
+      <c r="M29" s="25"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="26" t="s">
@@ -4939,7 +4924,7 @@
       <c r="L30" s="15" t="s">
         <v>311</v>
       </c>
-      <c r="M30" s="23" t="s">
+      <c r="M30" s="24" t="s">
         <v>311</v>
       </c>
     </row>
@@ -4962,7 +4947,7 @@
       <c r="L31" s="15" t="s">
         <v>311</v>
       </c>
-      <c r="M31" s="22"/>
+      <c r="M31" s="25"/>
     </row>
     <row r="32" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="26"/>
@@ -4983,7 +4968,7 @@
       <c r="L32" s="15" t="s">
         <v>311</v>
       </c>
-      <c r="M32" s="22"/>
+      <c r="M32" s="25"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="26"/>
@@ -5002,7 +4987,7 @@
       <c r="L33" s="15" t="s">
         <v>333</v>
       </c>
-      <c r="M33" s="22"/>
+      <c r="M33" s="25"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="26"/>
@@ -5021,7 +5006,7 @@
       <c r="L34" s="15" t="s">
         <v>336</v>
       </c>
-      <c r="M34" s="22"/>
+      <c r="M34" s="25"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="26"/>
@@ -5036,7 +5021,7 @@
       <c r="J35" s="15"/>
       <c r="K35" s="1"/>
       <c r="L35" s="15"/>
-      <c r="M35" s="22"/>
+      <c r="M35" s="25"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="26"/>
@@ -5051,7 +5036,7 @@
       <c r="J36" s="15"/>
       <c r="K36" s="1"/>
       <c r="L36" s="15"/>
-      <c r="M36" s="22"/>
+      <c r="M36" s="25"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="26"/>
@@ -5065,7 +5050,7 @@
       <c r="J37" s="15"/>
       <c r="K37" s="1"/>
       <c r="L37" s="15"/>
-      <c r="M37" s="22"/>
+      <c r="M37" s="25"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="26" t="s">
@@ -5092,7 +5077,7 @@
       <c r="L38" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="M38" s="23" t="s">
+      <c r="M38" s="24" t="s">
         <v>312</v>
       </c>
     </row>
@@ -5109,7 +5094,7 @@
       <c r="J39" s="15"/>
       <c r="K39" s="1"/>
       <c r="L39" s="15"/>
-      <c r="M39" s="22"/>
+      <c r="M39" s="25"/>
     </row>
     <row r="40" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="26" t="s">
@@ -5133,7 +5118,7 @@
       <c r="L40" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="M40" s="23" t="s">
+      <c r="M40" s="24" t="s">
         <v>313</v>
       </c>
     </row>
@@ -5151,7 +5136,7 @@
       <c r="L41" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="M41" s="22"/>
+      <c r="M41" s="25"/>
     </row>
     <row r="42" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="26"/>
@@ -5172,7 +5157,7 @@
       <c r="L42" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="M42" s="22"/>
+      <c r="M42" s="25"/>
     </row>
     <row r="43" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="26"/>
@@ -5192,7 +5177,7 @@
       <c r="L43" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="M43" s="22"/>
+      <c r="M43" s="25"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="26"/>
@@ -5211,7 +5196,7 @@
       <c r="L44" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="M44" s="22"/>
+      <c r="M44" s="25"/>
     </row>
     <row r="45" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A45" s="26"/>
@@ -5225,14 +5210,14 @@
         <v>338</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="7"/>
       <c r="K45" s="1"/>
       <c r="L45" s="15"/>
-      <c r="M45" s="22"/>
+      <c r="M45" s="25"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="26"/>
@@ -5244,7 +5229,7 @@
       <c r="I46" s="1"/>
       <c r="J46" s="7"/>
       <c r="L46" s="15"/>
-      <c r="M46" s="22"/>
+      <c r="M46" s="25"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="26"/>
@@ -5256,7 +5241,7 @@
       <c r="I47" s="1"/>
       <c r="J47" s="7"/>
       <c r="L47" s="15"/>
-      <c r="M47" s="22"/>
+      <c r="M47" s="25"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="26"/>
@@ -5268,7 +5253,7 @@
       <c r="I48" s="1"/>
       <c r="J48" s="7"/>
       <c r="L48" s="15"/>
-      <c r="M48" s="22"/>
+      <c r="M48" s="25"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="26"/>
@@ -5280,7 +5265,7 @@
       <c r="I49" s="1"/>
       <c r="J49" s="7"/>
       <c r="L49" s="15"/>
-      <c r="M49" s="22"/>
+      <c r="M49" s="25"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="26"/>
@@ -5292,7 +5277,7 @@
       <c r="I50" s="1"/>
       <c r="J50" s="7"/>
       <c r="L50" s="15"/>
-      <c r="M50" s="22"/>
+      <c r="M50" s="25"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="26"/>
@@ -5304,7 +5289,7 @@
       <c r="I51" s="1"/>
       <c r="J51" s="7"/>
       <c r="L51" s="15"/>
-      <c r="M51" s="22"/>
+      <c r="M51" s="25"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="26"/>
@@ -5316,7 +5301,7 @@
       <c r="I52" s="1"/>
       <c r="J52" s="7"/>
       <c r="L52" s="15"/>
-      <c r="M52" s="22"/>
+      <c r="M52" s="25"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="26"/>
@@ -5328,7 +5313,7 @@
       <c r="I53" s="1"/>
       <c r="J53" s="7"/>
       <c r="L53" s="15"/>
-      <c r="M53" s="22"/>
+      <c r="M53" s="25"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="26"/>
@@ -5340,7 +5325,7 @@
       <c r="I54" s="1"/>
       <c r="J54" s="7"/>
       <c r="L54" s="15"/>
-      <c r="M54" s="22"/>
+      <c r="M54" s="25"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="26" t="s">
@@ -5362,7 +5347,7 @@
       <c r="L55" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M55" s="32" t="s">
+      <c r="M55" s="31" t="s">
         <v>315</v>
       </c>
     </row>
@@ -5380,7 +5365,7 @@
       <c r="L56" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M56" s="22"/>
+      <c r="M56" s="25"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="26"/>
@@ -5398,7 +5383,7 @@
       <c r="L57" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M57" s="22"/>
+      <c r="M57" s="25"/>
     </row>
     <row r="58" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A58" s="26"/>
@@ -5416,7 +5401,7 @@
       <c r="L58" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M58" s="22"/>
+      <c r="M58" s="25"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="26"/>
@@ -5428,7 +5413,7 @@
       <c r="I59" s="1"/>
       <c r="J59" s="7"/>
       <c r="L59" s="15"/>
-      <c r="M59" s="22"/>
+      <c r="M59" s="25"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="26"/>
@@ -5440,7 +5425,7 @@
       <c r="I60" s="1"/>
       <c r="J60" s="7"/>
       <c r="L60" s="15"/>
-      <c r="M60" s="22"/>
+      <c r="M60" s="25"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="26"/>
@@ -5452,7 +5437,7 @@
       <c r="I61" s="1"/>
       <c r="J61" s="7"/>
       <c r="L61" s="15"/>
-      <c r="M61" s="22"/>
+      <c r="M61" s="25"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="26"/>
@@ -5464,7 +5449,7 @@
       <c r="I62" s="1"/>
       <c r="J62" s="7"/>
       <c r="L62" s="15"/>
-      <c r="M62" s="22"/>
+      <c r="M62" s="25"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="26"/>
@@ -5476,7 +5461,7 @@
       <c r="I63" s="1"/>
       <c r="J63" s="7"/>
       <c r="L63" s="15"/>
-      <c r="M63" s="22"/>
+      <c r="M63" s="25"/>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="26"/>
@@ -5487,7 +5472,7 @@
       <c r="F64" s="1"/>
       <c r="J64" s="7"/>
       <c r="L64" s="15"/>
-      <c r="M64" s="22"/>
+      <c r="M64" s="25"/>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="26" t="s">
@@ -5511,7 +5496,7 @@
       <c r="L65" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M65" s="32" t="s">
+      <c r="M65" s="31" t="s">
         <v>316</v>
       </c>
     </row>
@@ -5525,7 +5510,7 @@
       <c r="I66" s="1"/>
       <c r="J66" s="7"/>
       <c r="L66" s="15"/>
-      <c r="M66" s="22"/>
+      <c r="M66" s="25"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="26"/>
@@ -5537,7 +5522,7 @@
       <c r="I67" s="1"/>
       <c r="J67" s="7"/>
       <c r="L67" s="15"/>
-      <c r="M67" s="22"/>
+      <c r="M67" s="25"/>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="26"/>
@@ -5549,7 +5534,7 @@
       <c r="I68" s="1"/>
       <c r="J68" s="7"/>
       <c r="L68" s="15"/>
-      <c r="M68" s="22"/>
+      <c r="M68" s="25"/>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="26" t="s">
@@ -5573,14 +5558,14 @@
       <c r="L69" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M69" s="23" t="s">
+      <c r="M69" s="24" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="70" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="26"/>
-      <c r="B70" s="22"/>
-      <c r="C70" s="22"/>
+      <c r="B70" s="25"/>
+      <c r="C70" s="25"/>
       <c r="D70" s="1" t="s">
         <v>127</v>
       </c>
@@ -5594,12 +5579,12 @@
       <c r="L70" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M70" s="22"/>
+      <c r="M70" s="25"/>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="26"/>
-      <c r="B71" s="22"/>
-      <c r="C71" s="22"/>
+      <c r="B71" s="25"/>
+      <c r="C71" s="25"/>
       <c r="D71" s="1" t="s">
         <v>128</v>
       </c>
@@ -5611,12 +5596,12 @@
       <c r="L71" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M71" s="22"/>
+      <c r="M71" s="25"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="26"/>
-      <c r="B72" s="22"/>
-      <c r="C72" s="22"/>
+      <c r="B72" s="25"/>
+      <c r="C72" s="25"/>
       <c r="D72" s="1" t="s">
         <v>277</v>
       </c>
@@ -5627,12 +5612,12 @@
       <c r="L72" s="15" t="s">
         <v>309</v>
       </c>
-      <c r="M72" s="22"/>
+      <c r="M72" s="25"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="26"/>
-      <c r="B73" s="22"/>
-      <c r="C73" s="22"/>
+      <c r="B73" s="25"/>
+      <c r="C73" s="25"/>
       <c r="D73" s="1" t="s">
         <v>307</v>
       </c>
@@ -5643,38 +5628,38 @@
       <c r="L73" s="14" t="s">
         <v>314</v>
       </c>
-      <c r="M73" s="22"/>
+      <c r="M73" s="25"/>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="26"/>
-      <c r="B74" s="22"/>
-      <c r="C74" s="22"/>
+      <c r="B74" s="25"/>
+      <c r="C74" s="25"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="I74" s="1"/>
       <c r="J74" s="7"/>
       <c r="L74" s="15"/>
-      <c r="M74" s="22"/>
+      <c r="M74" s="25"/>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="26"/>
-      <c r="B75" s="22"/>
-      <c r="C75" s="22"/>
+      <c r="B75" s="25"/>
+      <c r="C75" s="25"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="I75" s="1"/>
       <c r="J75" s="7"/>
       <c r="L75" s="15"/>
-      <c r="M75" s="22"/>
+      <c r="M75" s="25"/>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="26"/>
-      <c r="B76" s="22"/>
-      <c r="C76" s="22"/>
+      <c r="B76" s="25"/>
+      <c r="C76" s="25"/>
       <c r="F76" s="1"/>
-      <c r="M76" s="22"/>
+      <c r="M76" s="25"/>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="26" t="s">
@@ -5698,7 +5683,7 @@
       <c r="L77" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M77" s="32" t="s">
+      <c r="M77" s="31" t="s">
         <v>315</v>
       </c>
     </row>
@@ -5716,7 +5701,7 @@
       <c r="L78" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M78" s="22"/>
+      <c r="M78" s="25"/>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="26" t="s">
@@ -5741,7 +5726,7 @@
       <c r="L79" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M79" s="32" t="s">
+      <c r="M79" s="31" t="s">
         <v>317</v>
       </c>
     </row>
@@ -5756,7 +5741,7 @@
       <c r="I80" s="1"/>
       <c r="J80" s="15"/>
       <c r="L80" s="15"/>
-      <c r="M80" s="22"/>
+      <c r="M80" s="25"/>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="26"/>
@@ -5768,7 +5753,7 @@
       <c r="I81" s="1"/>
       <c r="J81" s="15"/>
       <c r="L81" s="15"/>
-      <c r="M81" s="22"/>
+      <c r="M81" s="25"/>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="26"/>
@@ -5780,7 +5765,7 @@
       <c r="I82" s="1"/>
       <c r="J82" s="15"/>
       <c r="L82" s="15"/>
-      <c r="M82" s="22"/>
+      <c r="M82" s="25"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="26" t="s">
@@ -5849,14 +5834,14 @@
       <c r="L86" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M86" s="23" t="s">
+      <c r="M86" s="24" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" s="26"/>
-      <c r="B87" s="25"/>
-      <c r="C87" s="25"/>
+      <c r="B87" s="21"/>
+      <c r="C87" s="21"/>
       <c r="D87" s="1" t="s">
         <v>153</v>
       </c>
@@ -5867,55 +5852,55 @@
       <c r="L87" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M87" s="22"/>
+      <c r="M87" s="25"/>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" s="26"/>
-      <c r="B88" s="25"/>
-      <c r="C88" s="25"/>
+      <c r="B88" s="21"/>
+      <c r="C88" s="21"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="I88" s="1"/>
       <c r="J88" s="15"/>
       <c r="L88" s="15"/>
-      <c r="M88" s="22"/>
+      <c r="M88" s="25"/>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" s="26"/>
-      <c r="B89" s="25"/>
-      <c r="C89" s="25"/>
+      <c r="B89" s="21"/>
+      <c r="C89" s="21"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
       <c r="I89" s="1"/>
       <c r="J89" s="15"/>
       <c r="L89" s="15"/>
-      <c r="M89" s="22"/>
+      <c r="M89" s="25"/>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" s="26"/>
-      <c r="B90" s="25"/>
-      <c r="C90" s="25"/>
+      <c r="B90" s="21"/>
+      <c r="C90" s="21"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="I90" s="1"/>
       <c r="J90" s="15"/>
       <c r="L90" s="15"/>
-      <c r="M90" s="22"/>
+      <c r="M90" s="25"/>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" s="26"/>
-      <c r="B91" s="25"/>
-      <c r="C91" s="25"/>
+      <c r="B91" s="21"/>
+      <c r="C91" s="21"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
       <c r="I91" s="1"/>
       <c r="J91" s="15"/>
       <c r="L91" s="15"/>
-      <c r="M91" s="22"/>
+      <c r="M91" s="25"/>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
@@ -5983,14 +5968,52 @@
   </sheetData>
   <autoFilter ref="A1:M91" xr:uid="{FE8A9026-FDB0-4A8E-BB8F-FE98E3487D08}"/>
   <mergeCells count="70">
-    <mergeCell ref="C83:C85"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="L10:L12"/>
-    <mergeCell ref="K10:K12"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="C10:C16"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="M77:M78"/>
+    <mergeCell ref="M79:M82"/>
+    <mergeCell ref="M4:M8"/>
+    <mergeCell ref="M10:M16"/>
+    <mergeCell ref="M17:M25"/>
+    <mergeCell ref="M26:M29"/>
+    <mergeCell ref="M30:M37"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="A17:A25"/>
+    <mergeCell ref="A10:A16"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="C4:C9"/>
+    <mergeCell ref="B10:B16"/>
+    <mergeCell ref="M86:M91"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="M40:M54"/>
+    <mergeCell ref="M55:M64"/>
+    <mergeCell ref="M65:M68"/>
+    <mergeCell ref="M69:M76"/>
+    <mergeCell ref="B17:B25"/>
+    <mergeCell ref="C17:C25"/>
+    <mergeCell ref="F4:F8"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="D4:D8"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E4:E8"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="B30:B37"/>
+    <mergeCell ref="C30:C37"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A30:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A54"/>
+    <mergeCell ref="A55:A64"/>
+    <mergeCell ref="A69:A76"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="B86:B91"/>
+    <mergeCell ref="A83:A85"/>
     <mergeCell ref="C86:C91"/>
     <mergeCell ref="C77:C78"/>
     <mergeCell ref="B38:B39"/>
@@ -6007,52 +6030,14 @@
     <mergeCell ref="C69:C76"/>
     <mergeCell ref="B77:B78"/>
     <mergeCell ref="B83:B85"/>
-    <mergeCell ref="A69:A76"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="A79:A82"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="B86:B91"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="B30:B37"/>
-    <mergeCell ref="C30:C37"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A30:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A54"/>
-    <mergeCell ref="A55:A64"/>
-    <mergeCell ref="B17:B25"/>
-    <mergeCell ref="C17:C25"/>
-    <mergeCell ref="F4:F8"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="D4:D8"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="E4:E8"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="M86:M91"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="M40:M54"/>
-    <mergeCell ref="M55:M64"/>
-    <mergeCell ref="M65:M68"/>
-    <mergeCell ref="M69:M76"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="M77:M78"/>
-    <mergeCell ref="M79:M82"/>
-    <mergeCell ref="M4:M8"/>
-    <mergeCell ref="M10:M16"/>
-    <mergeCell ref="M17:M25"/>
-    <mergeCell ref="M26:M29"/>
-    <mergeCell ref="M30:M37"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="A17:A25"/>
-    <mergeCell ref="A10:A16"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="C4:C9"/>
-    <mergeCell ref="B10:B16"/>
+    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="L10:L12"/>
+    <mergeCell ref="K10:K12"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="C10:C16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M2" r:id="rId1" display="https://www.nuplazidhcp.com/about-pd-psychosis" xr:uid="{00000000-0004-0000-0200-000000000000}"/>

</xml_diff>

<commit_message>
Production Release 6th Aug 2024
</commit_message>
<xml_diff>
--- a/Corpus/MLR_Corpus.xlsx
+++ b/Corpus/MLR_Corpus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SivanSpeed\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CleverBrain\Nuplazid\Masori-Chatbot-UAT\Corpus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F2295B-2054-4519-B493-AE79EBC8BD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D91E44-F684-4A6E-884A-2A70C870B857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nuplazid Consumer" sheetId="3" r:id="rId1"/>
@@ -46,15 +46,7 @@
   <commentList>
     <comment ref="A2" authorId="0" shapeId="0" xr:uid="{7863A5D1-9B4B-42AA-9E3A-EFD2CA1F4ACC}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Are we missing Personal Stories and Talking to Healthcare Provider?
@@ -64,145 +56,72 @@
 - Speaking to a doctor 
 - or Speaking to a healthcare provider
 stuff like that. The site content will offer some better and more creative suggestions. I also understand that these aren't terms that people generally search for in SEM but if the goal is to help patients/caregivers better naviagate the site, those two pages usually have high engagement.</t>
-        </r>
       </text>
     </comment>
     <comment ref="C2" authorId="1" shapeId="0" xr:uid="{E64DB1B2-189A-48BC-A2B1-134AFAF4CC9B}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     What are delusions? What are hallucinations?
 Reply:
     I know more info is in the response and further down in the H&amp;D section but I think before people ask the second question, they may want to know what hallucinations and delusions are first as most people cannot define them</t>
-        </r>
       </text>
     </comment>
     <comment ref="F2" authorId="2" shapeId="0" xr:uid="{7D77409F-1EAA-44C8-96B2-9ED33BE485CA}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Provide link to information on site in response</t>
-        </r>
       </text>
     </comment>
     <comment ref="F3" authorId="3" shapeId="0" xr:uid="{7A10A0C6-BB3F-408D-A4EF-B3CB00342EF2}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Provide link to information on site in response</t>
-        </r>
       </text>
     </comment>
     <comment ref="F4" authorId="4" shapeId="0" xr:uid="{50AA08B8-0148-4B06-9956-D51213AE6275}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Provide link to information on site in response</t>
-        </r>
       </text>
     </comment>
     <comment ref="B5" authorId="5" shapeId="0" xr:uid="{DFB3A94E-DDA4-466E-AAE1-2757AB1D255D}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     MLR will make you remove this as we are only indicated in the US.</t>
-        </r>
       </text>
     </comment>
     <comment ref="C15" authorId="6" shapeId="0" xr:uid="{94516435-0266-4ADB-BEEF-4CB81A803132}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Where can I learn more? Something like that. We need to have something tied to email registrations.</t>
-        </r>
       </text>
     </comment>
     <comment ref="D25" authorId="7" shapeId="0" xr:uid="{422F338D-F43C-4C76-95CA-BE3FA3F1C9BA}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     I recommend to have "Acadia Connect and delete any mention of Nuplazid Connect.</t>
-        </r>
       </text>
     </comment>
     <comment ref="E27" authorId="8" shapeId="0" xr:uid="{6E745FC6-AE79-477C-95B8-95241C30BDC2}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     I recommend to have "Acadia Connect and delete any mention of Nuplazid Connect.</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -226,180 +145,90 @@
   <commentList>
     <comment ref="B4" authorId="0" shapeId="0" xr:uid="{1F2FC693-4862-4100-B58E-7C41F18A8E99}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Nuplazid indication
 patient resources</t>
-        </r>
       </text>
     </comment>
     <comment ref="C10" authorId="1" shapeId="0" xr:uid="{99EA3807-EB10-4FD7-896A-99B320C5B2E2}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     MLR may be concerned with the KOL question. The question posed back will be, "what response do they give if they type that in, given that we don't have any KOL opinions on site." I think this may be changing in the next few months. I'm not sure. Please check with Jake.
 Reply:
     I would delete that KOL question as we don't have any information on the site</t>
-        </r>
       </text>
     </comment>
     <comment ref="F10" authorId="2" shapeId="0" xr:uid="{E98F849F-AA15-47D7-8E3E-AF2E28183101}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Instead of just "only" please revise to "first and only" we say this on the HCP side of things but not on the consumer side.</t>
-        </r>
       </text>
     </comment>
     <comment ref="B17" authorId="3" shapeId="0" xr:uid="{B3A64F05-BDA5-47FC-9B9A-CF3ECAC976B8}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Nuplazid primary endpoint
 Nuplazid secondary endpoint</t>
-        </r>
       </text>
     </comment>
     <comment ref="C26" authorId="4" shapeId="0" xr:uid="{DE93CD08-8D71-480E-AF2B-94A4EDC1EACB}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     For consistency purposes, do we want to revise to "How are delusions measured?"</t>
-        </r>
       </text>
     </comment>
     <comment ref="B30" authorId="5" shapeId="0" xr:uid="{A0649205-201E-40CA-A513-834EE1E2B9FE}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     long-term safety
 drug interactions
 adverse reaction/event</t>
-        </r>
       </text>
     </comment>
     <comment ref="B40" authorId="6" shapeId="0" xr:uid="{490A6B21-E3F0-4BE3-84FA-875C273D4644}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     sprinkle
 dosing guide</t>
-        </r>
       </text>
     </comment>
     <comment ref="B65" authorId="7" shapeId="0" xr:uid="{A0B2C671-E543-4112-8919-FE70430826C8}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     forms</t>
-        </r>
       </text>
     </comment>
     <comment ref="C65" authorId="8" shapeId="0" xr:uid="{D9094AEA-42EA-4E64-8A3F-367796AF3240}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Remove Acadia?</t>
-        </r>
       </text>
     </comment>
     <comment ref="B69" authorId="9" shapeId="0" xr:uid="{5E44F182-AC11-45F7-AC37-DB904E84DBEC}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     coverage
 samples</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -407,7 +236,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="350">
   <si>
     <t>Keywords</t>
   </si>
@@ -1621,6 +1450,24 @@
   </si>
   <si>
     <t>/resources#FindSpecialist</t>
+  </si>
+  <si>
+    <t>Real-World Evidence</t>
+  </si>
+  <si>
+    <t>Real World Data, Mortality Data, Mosholder Study, Layton Study</t>
+  </si>
+  <si>
+    <t>real-world-evidence</t>
+  </si>
+  <si>
+    <t>Expert Perspectives</t>
+  </si>
+  <si>
+    <t>Expert Perspectives Videos, Specialist Videos, PD Psychosis Conversations Video, Initiating Treatment Video, Evidence for NUPLAZID® Video, Acadia Connect® Video</t>
+  </si>
+  <si>
+    <t>expert-perspectives</t>
   </si>
 </sst>
 </file>
@@ -2181,28 +2028,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.44140625" customWidth="1"/>
-    <col min="2" max="2" width="27.109375" customWidth="1"/>
-    <col min="3" max="3" width="47.109375" customWidth="1"/>
-    <col min="4" max="5" width="41.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="43.109375" customWidth="1"/>
-    <col min="7" max="7" width="34.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="47.140625" customWidth="1"/>
+    <col min="4" max="5" width="41.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="43.140625" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" customWidth="1"/>
-    <col min="12" max="12" width="37.33203125" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="37.28515625" customWidth="1"/>
     <col min="13" max="13" width="74" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -2243,7 +2090,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>200</v>
       </c>
@@ -2272,7 +2119,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -2293,7 +2140,7 @@
       </c>
       <c r="M3" s="25"/>
     </row>
-    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="21"/>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
@@ -2314,7 +2161,7 @@
       </c>
       <c r="M4" s="25"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>172</v>
       </c>
@@ -2343,7 +2190,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="23"/>
       <c r="B6" s="23"/>
       <c r="C6" s="23"/>
@@ -2364,7 +2211,7 @@
       </c>
       <c r="M6" s="25"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>255</v>
       </c>
@@ -2393,7 +2240,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -2414,7 +2261,7 @@
       </c>
       <c r="M8" s="25"/>
     </row>
-    <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
@@ -2432,7 +2279,7 @@
       </c>
       <c r="M9" s="25"/>
     </row>
-    <row r="10" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -2450,7 +2297,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="13"/>
     </row>
-    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>261</v>
       </c>
@@ -2476,7 +2323,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2489,7 +2336,7 @@
       <c r="L12" s="1"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2502,7 +2349,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="13"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2515,7 +2362,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>173</v>
       </c>
@@ -2544,7 +2391,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="23"/>
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
@@ -2565,7 +2412,7 @@
       </c>
       <c r="M16" s="25"/>
     </row>
-    <row r="17" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="23"/>
       <c r="B17" s="23"/>
       <c r="C17" s="23"/>
@@ -2586,7 +2433,7 @@
       </c>
       <c r="M17" s="25"/>
     </row>
-    <row r="18" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="23"/>
       <c r="B18" s="23"/>
       <c r="C18" s="23"/>
@@ -2603,7 +2450,7 @@
       <c r="L18" s="15"/>
       <c r="M18" s="25"/>
     </row>
-    <row r="19" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
         <v>174</v>
       </c>
@@ -2632,7 +2479,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="23"/>
       <c r="B20" s="21"/>
       <c r="C20" s="23"/>
@@ -2653,7 +2500,7 @@
       </c>
       <c r="M20" s="25"/>
     </row>
-    <row r="21" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="23"/>
       <c r="B21" s="21"/>
       <c r="C21" s="23"/>
@@ -2674,7 +2521,7 @@
       </c>
       <c r="M21" s="25"/>
     </row>
-    <row r="22" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="23"/>
       <c r="B22" s="21"/>
       <c r="C22" s="23"/>
@@ -2695,7 +2542,7 @@
       </c>
       <c r="M22" s="25"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
         <v>177</v>
       </c>
@@ -2721,7 +2568,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
       <c r="B24" s="21"/>
       <c r="C24" s="23"/>
@@ -2742,7 +2589,7 @@
       </c>
       <c r="M24" s="25"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="23"/>
       <c r="B25" s="21"/>
       <c r="C25" s="23"/>
@@ -2762,7 +2609,7 @@
       </c>
       <c r="M25" s="25"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="23"/>
       <c r="B26" s="21"/>
       <c r="C26" s="23"/>
@@ -2783,7 +2630,7 @@
       </c>
       <c r="M26" s="25"/>
     </row>
-    <row r="27" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>178</v>
       </c>
@@ -2811,7 +2658,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="23"/>
       <c r="B28" s="21"/>
       <c r="C28" s="26"/>
@@ -2832,7 +2679,7 @@
       </c>
       <c r="M28" s="25"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="23"/>
       <c r="B29" s="21"/>
       <c r="C29" s="26"/>
@@ -2841,7 +2688,7 @@
       </c>
       <c r="M29" s="25"/>
     </row>
-    <row r="30" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
         <v>180</v>
       </c>
@@ -2862,7 +2709,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="23"/>
       <c r="B31" s="21" t="s">
         <v>212</v>
@@ -2887,7 +2734,7 @@
       </c>
       <c r="M31" s="25"/>
     </row>
-    <row r="32" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="23"/>
       <c r="B32" s="23"/>
       <c r="C32" s="21"/>
@@ -2907,7 +2754,7 @@
       <c r="L32" s="15"/>
       <c r="M32" s="25"/>
     </row>
-    <row r="33" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="23"/>
       <c r="B33" s="23"/>
       <c r="C33" s="21"/>
@@ -2925,7 +2772,7 @@
       </c>
       <c r="M33" s="25"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="23"/>
       <c r="B34" s="23"/>
       <c r="C34" s="21"/>
@@ -2946,7 +2793,7 @@
       </c>
       <c r="M34" s="25"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="23"/>
       <c r="B35" s="23"/>
       <c r="C35" s="21"/>
@@ -2967,7 +2814,7 @@
       </c>
       <c r="M35" s="25"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="23"/>
       <c r="B36" s="23"/>
       <c r="C36" s="21"/>
@@ -2985,7 +2832,7 @@
       </c>
       <c r="M36" s="25"/>
     </row>
-    <row r="37" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
         <v>214</v>
       </c>
@@ -3014,7 +2861,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="21"/>
       <c r="B38" s="21"/>
       <c r="C38" s="23"/>
@@ -3035,7 +2882,7 @@
       </c>
       <c r="M38" s="25"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="23"/>
@@ -3048,7 +2895,7 @@
       </c>
       <c r="M39" s="25"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="21"/>
       <c r="B40" s="21"/>
       <c r="C40" s="23"/>
@@ -3060,7 +2907,7 @@
       </c>
       <c r="M40" s="25"/>
     </row>
-    <row r="41" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="21"/>
       <c r="B41" s="21"/>
       <c r="C41" s="23"/>
@@ -3081,7 +2928,7 @@
       </c>
       <c r="M41" s="25"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="21"/>
       <c r="B42" s="21"/>
       <c r="C42" s="23"/>
@@ -3102,7 +2949,7 @@
       </c>
       <c r="M42" s="25"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="21"/>
       <c r="B43" s="21"/>
       <c r="C43" s="23"/>
@@ -3123,7 +2970,7 @@
       </c>
       <c r="M43" s="25"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="F44" s="1"/>
@@ -3135,7 +2982,7 @@
       <c r="L44" s="1"/>
       <c r="M44" s="13"/>
     </row>
-    <row r="45" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>189</v>
       </c>
@@ -3159,7 +3006,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>342</v>
       </c>
@@ -3272,15 +3119,15 @@
       <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.6640625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
-    <col min="4" max="4" width="95.33203125" customWidth="1"/>
+    <col min="1" max="2" width="20.7109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="95.28515625" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -3297,7 +3144,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>2</v>
       </c>
@@ -3312,7 +3159,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="29"/>
       <c r="B3" s="10"/>
       <c r="C3" t="s">
@@ -3321,7 +3168,7 @@
       <c r="D3" s="4"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="29"/>
       <c r="B4" s="10"/>
       <c r="C4" t="s">
@@ -3330,7 +3177,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
       <c r="B5" s="10"/>
       <c r="C5" t="s">
@@ -3339,7 +3186,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="29"/>
       <c r="B6" s="10"/>
       <c r="C6" t="s">
@@ -3348,7 +3195,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="29"/>
       <c r="B7" s="10"/>
       <c r="C7" t="s">
@@ -3357,7 +3204,7 @@
       <c r="D7" s="4"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="29"/>
       <c r="B8" s="10"/>
       <c r="C8" t="s">
@@ -3366,7 +3213,7 @@
       <c r="D8" s="4"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="29"/>
       <c r="B9" s="10"/>
       <c r="C9" t="s">
@@ -3375,7 +3222,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="29"/>
       <c r="B10" s="10"/>
       <c r="C10" t="s">
@@ -3384,7 +3231,7 @@
       <c r="D10" s="4"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>16</v>
       </c>
@@ -3393,28 +3240,28 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="29"/>
       <c r="B12" s="10"/>
       <c r="C12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="29"/>
       <c r="B13" s="10"/>
       <c r="C13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="29"/>
       <c r="B14" s="10"/>
       <c r="C14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="29"/>
       <c r="B15" s="10"/>
       <c r="C15" t="s">
@@ -3424,7 +3271,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="29"/>
       <c r="B16" s="10"/>
       <c r="C16" t="s">
@@ -3434,7 +3281,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
         <v>23</v>
       </c>
@@ -3449,7 +3296,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="29"/>
       <c r="B18" s="10"/>
       <c r="C18" t="s">
@@ -3459,21 +3306,21 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="29"/>
       <c r="B19" s="10"/>
       <c r="C19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="29"/>
       <c r="B20" s="10"/>
       <c r="C20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="29"/>
       <c r="B21" s="10"/>
       <c r="C21" t="s">
@@ -3483,7 +3330,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="29"/>
       <c r="B22" s="10"/>
       <c r="C22" t="s">
@@ -3493,7 +3340,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
       <c r="B23" s="10"/>
       <c r="C23" t="s">
@@ -3503,14 +3350,14 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="29"/>
       <c r="B24" s="10"/>
       <c r="C24" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
         <v>41</v>
       </c>
@@ -3525,7 +3372,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="29"/>
       <c r="B26" s="10"/>
       <c r="C26" t="s">
@@ -3535,7 +3382,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="29"/>
       <c r="B27" s="10"/>
       <c r="C27" t="s">
@@ -3545,7 +3392,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="29"/>
       <c r="B28" s="10"/>
       <c r="C28" t="s">
@@ -3555,7 +3402,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="29"/>
       <c r="B29" s="10"/>
       <c r="C29" t="s">
@@ -3565,7 +3412,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="29"/>
       <c r="B30" s="10"/>
       <c r="C30" t="s">
@@ -3575,49 +3422,49 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="29"/>
       <c r="B31" s="10"/>
       <c r="D31" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="29"/>
       <c r="B32" s="10"/>
       <c r="D32" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="29"/>
       <c r="B33" s="10"/>
       <c r="D33" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="29"/>
       <c r="B34" s="10"/>
       <c r="D34" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="29"/>
       <c r="B35" s="10"/>
       <c r="D35" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="29"/>
       <c r="B36" s="10"/>
       <c r="D36" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
         <v>58</v>
       </c>
@@ -3625,43 +3472,43 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="26"/>
       <c r="D38" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="26"/>
       <c r="D39" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="26"/>
       <c r="D40" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="26"/>
       <c r="D41" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="26"/>
       <c r="D42" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="26"/>
       <c r="D43" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="26" t="s">
         <v>66</v>
       </c>
@@ -3672,7 +3519,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="26"/>
       <c r="C45" t="s">
         <v>67</v>
@@ -3681,7 +3528,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="26"/>
       <c r="C46" t="s">
         <v>44</v>
@@ -3690,43 +3537,43 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="26"/>
       <c r="D47" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="26"/>
       <c r="D48" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="26"/>
       <c r="D49" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="26"/>
       <c r="D50" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="26"/>
       <c r="D51" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="26"/>
       <c r="D52" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="158.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="158.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="26" t="s">
         <v>77</v>
       </c>
@@ -3737,7 +3584,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="26"/>
       <c r="C54" t="s">
         <v>87</v>
@@ -3746,7 +3593,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="26" t="s">
         <v>80</v>
       </c>
@@ -3757,7 +3604,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="26"/>
       <c r="C56" t="s">
         <v>82</v>
@@ -3766,7 +3613,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="26"/>
       <c r="C57" t="s">
         <v>83</v>
@@ -3775,7 +3622,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="26"/>
       <c r="C58" t="s">
         <v>84</v>
@@ -3784,7 +3631,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="26"/>
       <c r="C59" t="s">
         <v>85</v>
@@ -3793,73 +3640,73 @@
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="26"/>
       <c r="D60" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="26"/>
       <c r="D61" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="26"/>
       <c r="D62" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="26"/>
       <c r="D63" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="26"/>
       <c r="D64" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="26"/>
       <c r="D65" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="26"/>
       <c r="D66" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="26"/>
       <c r="D67" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="26"/>
       <c r="D68" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="26"/>
       <c r="D69" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="26"/>
       <c r="D70" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="26" t="s">
         <v>104</v>
       </c>
@@ -3870,7 +3717,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="26"/>
       <c r="C72" t="s">
         <v>106</v>
@@ -3879,7 +3726,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="26"/>
       <c r="C73" t="s">
         <v>107</v>
@@ -3888,7 +3735,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="26"/>
       <c r="C74" t="s">
         <v>108</v>
@@ -3897,43 +3744,43 @@
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="26"/>
       <c r="D75" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="26"/>
       <c r="D76" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="26"/>
       <c r="D77" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="26"/>
       <c r="D78" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="26"/>
       <c r="D79" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="26"/>
       <c r="D80" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="26" t="s">
         <v>117</v>
       </c>
@@ -3944,7 +3791,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="26"/>
       <c r="C82" t="s">
         <v>119</v>
@@ -3953,7 +3800,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="26"/>
       <c r="C83" t="s">
         <v>120</v>
@@ -3962,25 +3809,25 @@
         <v>122</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="26"/>
       <c r="D84" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="26"/>
       <c r="D85" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="26"/>
       <c r="D86" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="26" t="s">
         <v>125</v>
       </c>
@@ -3991,7 +3838,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" s="26"/>
       <c r="C88" t="s">
         <v>127</v>
@@ -4000,7 +3847,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" s="26"/>
       <c r="C89" t="s">
         <v>128</v>
@@ -4009,13 +3856,13 @@
         <v>131</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="26"/>
       <c r="C90" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" s="26" t="s">
         <v>132</v>
       </c>
@@ -4026,7 +3873,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A92" s="26"/>
       <c r="C92" t="s">
         <v>134</v>
@@ -4035,37 +3882,37 @@
         <v>140</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="26"/>
       <c r="C93" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="26"/>
       <c r="C94" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="26"/>
       <c r="C95" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="26"/>
       <c r="C96" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="26"/>
       <c r="C97" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="26" t="s">
         <v>141</v>
       </c>
@@ -4073,25 +3920,25 @@
         <v>142</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="26"/>
       <c r="D99" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="26"/>
       <c r="D100" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="26"/>
       <c r="D101" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="26" t="s">
         <v>146</v>
       </c>
@@ -4102,7 +3949,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="26"/>
       <c r="C103" t="s">
         <v>138</v>
@@ -4111,7 +3958,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="26"/>
       <c r="C104" t="s">
         <v>135</v>
@@ -4120,7 +3967,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="26"/>
       <c r="C105" t="s">
         <v>147</v>
@@ -4129,7 +3976,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="26"/>
       <c r="C106" t="s">
         <v>148</v>
@@ -4138,13 +3985,13 @@
         <v>123</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="26"/>
       <c r="C107" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="26" t="s">
         <v>151</v>
       </c>
@@ -4155,7 +4002,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="26"/>
       <c r="C109" t="s">
         <v>153</v>
@@ -4164,31 +4011,31 @@
         <v>112</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="26"/>
       <c r="D110" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="26"/>
       <c r="D111" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="26"/>
       <c r="D112" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="26"/>
       <c r="D113" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="26" t="s">
         <v>163</v>
       </c>
@@ -4199,7 +4046,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="26"/>
       <c r="C115" t="s">
         <v>119</v>
@@ -4208,7 +4055,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="26"/>
       <c r="C116" t="s">
         <v>120</v>
@@ -4217,55 +4064,55 @@
         <v>160</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="26"/>
       <c r="D117" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="26"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="26"/>
       <c r="D119" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="26"/>
       <c r="D120" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="26"/>
       <c r="D121" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="26"/>
       <c r="D122" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="26"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="26"/>
       <c r="D124" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A125" s="26"/>
       <c r="D125" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="26"/>
       <c r="D126" t="s">
         <v>170</v>
@@ -4304,27 +4151,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M100"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="2" width="47.33203125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="47.28515625" style="13" customWidth="1"/>
     <col min="3" max="3" width="44" style="13" customWidth="1"/>
-    <col min="4" max="4" width="36.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" customWidth="1"/>
-    <col min="7" max="7" width="31.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" customWidth="1"/>
-    <col min="9" max="11" width="37.33203125" customWidth="1"/>
-    <col min="12" max="12" width="37.33203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="52.44140625" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="11" width="37.28515625" customWidth="1"/>
+    <col min="12" max="12" width="37.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="52.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -4365,7 +4212,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>2</v>
       </c>
@@ -4394,7 +4241,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
@@ -4415,7 +4262,7 @@
       </c>
       <c r="M3" s="16"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>16</v>
       </c>
@@ -4444,7 +4291,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
       <c r="B5" s="26"/>
       <c r="C5" s="26"/>
@@ -4461,7 +4308,7 @@
       </c>
       <c r="M5" s="25"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="29"/>
       <c r="B6" s="26"/>
       <c r="C6" s="26"/>
@@ -4478,7 +4325,7 @@
       </c>
       <c r="M6" s="25"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="29"/>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -4495,7 +4342,7 @@
       </c>
       <c r="M7" s="25"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="29"/>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
@@ -4512,7 +4359,7 @@
       </c>
       <c r="M8" s="25"/>
     </row>
-    <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="29"/>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -4535,7 +4382,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>191</v>
       </c>
@@ -4564,7 +4411,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29"/>
       <c r="B11" s="21"/>
       <c r="C11" s="26"/>
@@ -4579,7 +4426,7 @@
       <c r="L11" s="31"/>
       <c r="M11" s="25"/>
     </row>
-    <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29"/>
       <c r="B12" s="21"/>
       <c r="C12" s="26"/>
@@ -4594,7 +4441,7 @@
       <c r="L12" s="31"/>
       <c r="M12" s="25"/>
     </row>
-    <row r="13" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="29"/>
       <c r="B13" s="21"/>
       <c r="C13" s="26"/>
@@ -4615,7 +4462,7 @@
       </c>
       <c r="M13" s="25"/>
     </row>
-    <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="29"/>
       <c r="B14" s="21"/>
       <c r="C14" s="26"/>
@@ -4636,7 +4483,7 @@
       </c>
       <c r="M14" s="25"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="29"/>
       <c r="B15" s="21"/>
       <c r="C15" s="26"/>
@@ -4651,7 +4498,7 @@
       <c r="L15" s="15"/>
       <c r="M15" s="25"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="29"/>
       <c r="B16" s="21"/>
       <c r="C16" s="26"/>
@@ -4666,7 +4513,7 @@
       <c r="L16" s="15"/>
       <c r="M16" s="25"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
         <v>41</v>
       </c>
@@ -4689,7 +4536,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="29"/>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
@@ -4704,7 +4551,7 @@
       <c r="L18" s="15"/>
       <c r="M18" s="24"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="29"/>
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
@@ -4716,7 +4563,7 @@
       <c r="L19" s="15"/>
       <c r="M19" s="24"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="29"/>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
@@ -4731,7 +4578,7 @@
       <c r="L20" s="15"/>
       <c r="M20" s="24"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="29"/>
       <c r="B21" s="26"/>
       <c r="C21" s="26"/>
@@ -4750,7 +4597,7 @@
       </c>
       <c r="M21" s="24"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="29"/>
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
@@ -4771,7 +4618,7 @@
       </c>
       <c r="M22" s="24"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
       <c r="B23" s="26"/>
       <c r="C23" s="26"/>
@@ -4787,7 +4634,7 @@
       </c>
       <c r="M23" s="24"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="29"/>
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
@@ -4808,7 +4655,7 @@
       </c>
       <c r="M24" s="24"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="29"/>
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
@@ -4825,7 +4672,7 @@
       </c>
       <c r="M25" s="24"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
         <v>58</v>
       </c>
@@ -4846,7 +4693,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
       <c r="B27" s="26"/>
       <c r="C27" s="26"/>
@@ -4867,7 +4714,7 @@
       </c>
       <c r="M27" s="25"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
       <c r="B28" s="26"/>
       <c r="C28" s="26"/>
@@ -4883,7 +4730,7 @@
       </c>
       <c r="M28" s="25"/>
     </row>
-    <row r="29" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="26"/>
       <c r="B29" s="26"/>
       <c r="C29" s="26"/>
@@ -4904,7 +4751,7 @@
       </c>
       <c r="M29" s="25"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
         <v>66</v>
       </c>
@@ -4928,7 +4775,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="26"/>
       <c r="B31" s="26"/>
       <c r="C31" s="26"/>
@@ -4949,7 +4796,7 @@
       </c>
       <c r="M31" s="25"/>
     </row>
-    <row r="32" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="26"/>
       <c r="B32" s="26"/>
       <c r="C32" s="26"/>
@@ -4970,7 +4817,7 @@
       </c>
       <c r="M32" s="25"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="26"/>
       <c r="B33" s="26"/>
       <c r="C33" s="26"/>
@@ -4989,7 +4836,7 @@
       </c>
       <c r="M33" s="25"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="26"/>
       <c r="B34" s="26"/>
       <c r="C34" s="26"/>
@@ -5008,7 +4855,7 @@
       </c>
       <c r="M34" s="25"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="26"/>
       <c r="B35" s="26"/>
       <c r="C35" s="26"/>
@@ -5023,7 +4870,7 @@
       <c r="L35" s="15"/>
       <c r="M35" s="25"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="26"/>
       <c r="B36" s="26"/>
       <c r="C36" s="26"/>
@@ -5038,7 +4885,7 @@
       <c r="L36" s="15"/>
       <c r="M36" s="25"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="26"/>
       <c r="B37" s="26"/>
       <c r="C37" s="26"/>
@@ -5052,7 +4899,7 @@
       <c r="L37" s="15"/>
       <c r="M37" s="25"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
         <v>77</v>
       </c>
@@ -5081,7 +4928,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
@@ -5096,7 +4943,7 @@
       <c r="L39" s="15"/>
       <c r="M39" s="25"/>
     </row>
-    <row r="40" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
         <v>80</v>
       </c>
@@ -5122,7 +4969,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="26"/>
       <c r="B41" s="26"/>
       <c r="C41" s="26"/>
@@ -5138,7 +4985,7 @@
       </c>
       <c r="M41" s="25"/>
     </row>
-    <row r="42" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="26"/>
       <c r="B42" s="26"/>
       <c r="C42" s="26"/>
@@ -5159,7 +5006,7 @@
       </c>
       <c r="M42" s="25"/>
     </row>
-    <row r="43" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="26"/>
       <c r="B43" s="26"/>
       <c r="C43" s="26"/>
@@ -5179,7 +5026,7 @@
       </c>
       <c r="M43" s="25"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="26"/>
       <c r="B44" s="26"/>
       <c r="C44" s="26"/>
@@ -5198,7 +5045,7 @@
       </c>
       <c r="M44" s="25"/>
     </row>
-    <row r="45" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="26"/>
       <c r="B45" s="26"/>
       <c r="C45" s="26"/>
@@ -5219,7 +5066,7 @@
       <c r="L45" s="15"/>
       <c r="M45" s="25"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="26"/>
       <c r="B46" s="26"/>
       <c r="C46" s="26"/>
@@ -5231,7 +5078,7 @@
       <c r="L46" s="15"/>
       <c r="M46" s="25"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="26"/>
       <c r="B47" s="26"/>
       <c r="C47" s="26"/>
@@ -5243,7 +5090,7 @@
       <c r="L47" s="15"/>
       <c r="M47" s="25"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="26"/>
       <c r="B48" s="26"/>
       <c r="C48" s="26"/>
@@ -5255,7 +5102,7 @@
       <c r="L48" s="15"/>
       <c r="M48" s="25"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="26"/>
       <c r="B49" s="26"/>
       <c r="C49" s="26"/>
@@ -5267,7 +5114,7 @@
       <c r="L49" s="15"/>
       <c r="M49" s="25"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="26"/>
       <c r="B50" s="26"/>
       <c r="C50" s="26"/>
@@ -5279,7 +5126,7 @@
       <c r="L50" s="15"/>
       <c r="M50" s="25"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="26"/>
       <c r="B51" s="26"/>
       <c r="C51" s="26"/>
@@ -5291,7 +5138,7 @@
       <c r="L51" s="15"/>
       <c r="M51" s="25"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="26"/>
       <c r="B52" s="26"/>
       <c r="C52" s="26"/>
@@ -5303,7 +5150,7 @@
       <c r="L52" s="15"/>
       <c r="M52" s="25"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="26"/>
       <c r="B53" s="26"/>
       <c r="C53" s="26"/>
@@ -5315,7 +5162,7 @@
       <c r="L53" s="15"/>
       <c r="M53" s="25"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="26"/>
       <c r="B54" s="26"/>
       <c r="C54" s="26"/>
@@ -5327,7 +5174,7 @@
       <c r="L54" s="15"/>
       <c r="M54" s="25"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="26" t="s">
         <v>183</v>
       </c>
@@ -5351,7 +5198,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="26"/>
       <c r="B56" s="26"/>
       <c r="C56" s="26"/>
@@ -5367,7 +5214,7 @@
       </c>
       <c r="M56" s="25"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="26"/>
       <c r="B57" s="26"/>
       <c r="C57" s="26"/>
@@ -5385,7 +5232,7 @@
       </c>
       <c r="M57" s="25"/>
     </row>
-    <row r="58" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="26"/>
       <c r="B58" s="26"/>
       <c r="C58" s="26"/>
@@ -5403,7 +5250,7 @@
       </c>
       <c r="M58" s="25"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="26"/>
       <c r="B59" s="26"/>
       <c r="C59" s="26"/>
@@ -5415,7 +5262,7 @@
       <c r="L59" s="15"/>
       <c r="M59" s="25"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="26"/>
       <c r="B60" s="26"/>
       <c r="C60" s="26"/>
@@ -5427,7 +5274,7 @@
       <c r="L60" s="15"/>
       <c r="M60" s="25"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="26"/>
       <c r="B61" s="26"/>
       <c r="C61" s="26"/>
@@ -5439,7 +5286,7 @@
       <c r="L61" s="15"/>
       <c r="M61" s="25"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="26"/>
       <c r="B62" s="26"/>
       <c r="C62" s="26"/>
@@ -5451,7 +5298,7 @@
       <c r="L62" s="15"/>
       <c r="M62" s="25"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="26"/>
       <c r="B63" s="26"/>
       <c r="C63" s="26"/>
@@ -5463,7 +5310,7 @@
       <c r="L63" s="15"/>
       <c r="M63" s="25"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="26"/>
       <c r="B64" s="26"/>
       <c r="C64" s="26"/>
@@ -5474,7 +5321,7 @@
       <c r="L64" s="15"/>
       <c r="M64" s="25"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="26" t="s">
         <v>117</v>
       </c>
@@ -5500,7 +5347,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="26"/>
       <c r="B66" s="26"/>
       <c r="C66" s="26"/>
@@ -5512,7 +5359,7 @@
       <c r="L66" s="15"/>
       <c r="M66" s="25"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="26"/>
       <c r="B67" s="26"/>
       <c r="C67" s="26"/>
@@ -5524,7 +5371,7 @@
       <c r="L67" s="15"/>
       <c r="M67" s="25"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="26"/>
       <c r="B68" s="26"/>
       <c r="C68" s="26"/>
@@ -5536,7 +5383,7 @@
       <c r="L68" s="15"/>
       <c r="M68" s="25"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="26" t="s">
         <v>125</v>
       </c>
@@ -5562,7 +5409,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="26"/>
       <c r="B70" s="25"/>
       <c r="C70" s="25"/>
@@ -5581,7 +5428,7 @@
       </c>
       <c r="M70" s="25"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="26"/>
       <c r="B71" s="25"/>
       <c r="C71" s="25"/>
@@ -5598,7 +5445,7 @@
       </c>
       <c r="M71" s="25"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="26"/>
       <c r="B72" s="25"/>
       <c r="C72" s="25"/>
@@ -5614,7 +5461,7 @@
       </c>
       <c r="M72" s="25"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="26"/>
       <c r="B73" s="25"/>
       <c r="C73" s="25"/>
@@ -5630,7 +5477,7 @@
       </c>
       <c r="M73" s="25"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="26"/>
       <c r="B74" s="25"/>
       <c r="C74" s="25"/>
@@ -5642,7 +5489,7 @@
       <c r="L74" s="15"/>
       <c r="M74" s="25"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="26"/>
       <c r="B75" s="25"/>
       <c r="C75" s="25"/>
@@ -5654,14 +5501,14 @@
       <c r="L75" s="15"/>
       <c r="M75" s="25"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="26"/>
       <c r="B76" s="25"/>
       <c r="C76" s="25"/>
       <c r="F76" s="1"/>
       <c r="M76" s="25"/>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="26" t="s">
         <v>132</v>
       </c>
@@ -5687,7 +5534,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="26"/>
       <c r="B78" s="26"/>
       <c r="C78" s="26"/>
@@ -5703,7 +5550,7 @@
       </c>
       <c r="M78" s="25"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="26" t="s">
         <v>141</v>
       </c>
@@ -5730,7 +5577,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="26"/>
       <c r="B80" s="26"/>
       <c r="C80" s="26"/>
@@ -5743,7 +5590,7 @@
       <c r="L80" s="15"/>
       <c r="M80" s="25"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="26"/>
       <c r="B81" s="26"/>
       <c r="C81" s="26"/>
@@ -5755,7 +5602,7 @@
       <c r="L81" s="15"/>
       <c r="M81" s="25"/>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="26"/>
       <c r="B82" s="26"/>
       <c r="C82" s="26"/>
@@ -5767,7 +5614,7 @@
       <c r="L82" s="15"/>
       <c r="M82" s="25"/>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="26" t="s">
         <v>146</v>
       </c>
@@ -5787,7 +5634,7 @@
       </c>
       <c r="M83" s="13"/>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="26"/>
       <c r="B84" s="26"/>
       <c r="C84" s="26"/>
@@ -5798,7 +5645,7 @@
       <c r="L84" s="15"/>
       <c r="M84" s="13"/>
     </row>
-    <row r="85" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="26"/>
       <c r="B85" s="26"/>
       <c r="C85" s="26"/>
@@ -5814,7 +5661,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="26" t="s">
         <v>233</v>
       </c>
@@ -5838,7 +5685,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="26"/>
       <c r="B87" s="21"/>
       <c r="C87" s="21"/>
@@ -5854,7 +5701,7 @@
       </c>
       <c r="M87" s="25"/>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="26"/>
       <c r="B88" s="21"/>
       <c r="C88" s="21"/>
@@ -5866,7 +5713,7 @@
       <c r="L88" s="15"/>
       <c r="M88" s="25"/>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="26"/>
       <c r="B89" s="21"/>
       <c r="C89" s="21"/>
@@ -5878,7 +5725,7 @@
       <c r="L89" s="15"/>
       <c r="M89" s="25"/>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="26"/>
       <c r="B90" s="21"/>
       <c r="C90" s="21"/>
@@ -5890,7 +5737,7 @@
       <c r="L90" s="15"/>
       <c r="M90" s="25"/>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="26"/>
       <c r="B91" s="21"/>
       <c r="C91" s="21"/>
@@ -5902,63 +5749,81 @@
       <c r="L91" s="15"/>
       <c r="M91" s="25"/>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
+    <row r="92" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>345</v>
+      </c>
       <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
+      <c r="D92" s="1" t="s">
+        <v>344</v>
+      </c>
       <c r="E92" s="1"/>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
+      <c r="L92" s="15" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>348</v>
+      </c>
       <c r="C93" s="1"/>
-      <c r="D93" s="1"/>
+      <c r="D93" s="1" t="s">
+        <v>347</v>
+      </c>
       <c r="E93" s="1"/>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L93" s="15" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -6085,9 +5950,11 @@
     <hyperlink ref="L86" r:id="rId43" display="https://nuplazidhcp-masori.azurewebsites.net/acadia-connect" xr:uid="{4156660E-63BE-4C9E-9BB0-07995FF24232}"/>
     <hyperlink ref="L71" r:id="rId44" display="https://nuplazidhcp-masori.azurewebsites.net/acadia-connect" xr:uid="{CC27EF93-F869-4B7A-8F92-4EAB845AFE74}"/>
     <hyperlink ref="L34" r:id="rId45" xr:uid="{7DB2A8E2-4CC8-4092-BEC6-58C2F9FF391A}"/>
+    <hyperlink ref="L92" r:id="rId46" xr:uid="{71B60A6B-63B8-44FB-BDB6-6CA5E82AB29D}"/>
+    <hyperlink ref="L93" r:id="rId47" xr:uid="{FBE13B3B-95C6-4B72-B3B3-165C1AB77157}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId46"/>
-  <legacyDrawing r:id="rId47"/>
+  <pageSetup orientation="portrait" r:id="rId48"/>
+  <legacyDrawing r:id="rId49"/>
 </worksheet>
 </file>
</xml_diff>